<commit_message>
PROS-5749 - CCRU - OSA new logic - deployment
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/Convenience Big PoS 2018.xlsx
+++ b/Projects/CCRU_SAND/Data/Convenience Big PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Convenience Big" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,6 +52,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1470,10 +1471,10 @@
     <t xml:space="preserve">CCH coolers quality (Prime Pos, Max15, Merch STD, Occupancy, Lights&amp;clean)</t>
   </si>
   <si>
-    <t xml:space="preserve">Cooler: Max 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Холодильники: Максимум 23 СКЮ на дверь</t>
+    <t xml:space="preserve">Cooler: Max 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Максимум 26 СКЮ на дверь</t>
   </si>
   <si>
     <t xml:space="preserve">number of SKU per Door RANGE</t>
@@ -1971,9 +1972,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="0%"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
@@ -2154,7 +2155,7 @@
     </border>
   </borders>
   <cellStyleXfs count="21">
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2176,43 +2177,99 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="49">
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2220,75 +2277,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2296,31 +2297,31 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2328,31 +2329,27 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2360,23 +2357,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2396,20 +2397,9 @@
         <name val="Calibri"/>
         <charset val="1"/>
         <family val="2"/>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
         <color rgb="FF000000"/>
-        <u val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="0%"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -2486,19 +2476,19 @@
   </sheetPr>
   <dimension ref="A1:AR184"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="AG149" activeCellId="0" sqref="AG149"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="M148" activeCellId="0" sqref="M148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="46.5951417004049"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="14.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="48.7044534412956"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="14.4251012145749"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="14.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="14.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="51.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15216,7 +15206,7 @@
         <v>1</v>
       </c>
       <c r="M147" s="12" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="N147" s="9" t="s">
         <v>242</v>
@@ -18352,9 +18342,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="37" t="s">
@@ -18389,9 +18376,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="39" t="s">
@@ -18521,9 +18505,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">

</xml_diff>